<commit_message>
wlconf: update wlconf_unit_test.xlsx to latest
Signed-off-by: Yair Shapira <yair.shapira@ti.com>
</commit_message>
<xml_diff>
--- a/wlconf/tests/wlconf_unit_test.xlsx
+++ b/wlconf/tests/wlconf_unit_test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="183">
   <si>
     <t>Category</t>
   </si>
@@ -1163,159 +1163,10 @@
     <t>Print the element tree structure with no data</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Run the following command:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>./wlconf -p &gt; tests/result-4.7.struct</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Then check that the output matches the pre-defined one:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>diff -u tests/result-4.7.struct tests/test-4.7.struct</t>
-    </r>
-  </si>
-  <si>
     <t>there should be no difference between the result-4.7.struct and test-4.7.struct files</t>
   </si>
   <si>
     <t>Getting values from default config file</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Make sure you have a valid input file (test-4.6-conf.bin) and run:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>./wlconf -g  &gt; tests/result-4.8-1.conf</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Then write the result back with the following command:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>./wlconf -C tests/result-4.8-1.conf -o tests/result-4.8-conf.bin</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-And read it again:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>./wlconf --get  &gt; tests/result-4.8-2.conf</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Compare the output text configuration files:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">diff -u tests/result-4.8-1.conf tests/result-4.8-2.conf
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Compare the deault and output configuration bin file:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>diff -ua wl18xx-conf-default.bin tests/result-4.8-conf.bin</t>
-    </r>
   </si>
   <si>
     <t>there should be no difference between the result-4.8-1.conf and result-4.8-2.conf files.
@@ -3439,10 +3290,6 @@
     <t>Tests should pass in all environments with same results</t>
   </si>
   <si>
-    <t>wlconf should run the same in multi systems - including with different word sizes, alignment, char signed/unsigned, etc…
-Currently the only limitation is that it should be used on Little Endians machines (such as ARM and X86)</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">the tool should reject the file and print an error:
 </t>
@@ -3522,19 +3369,274 @@
   </si>
   <si>
     <r>
-      <t>Remove bin configuration:
-r</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>m /system/etc/firmware/ti-connectivity/wl18xx-conf.bin</t>
+      <t xml:space="preserve">Run the following command:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>./wlconf -s core.hangover.quiet_time=0x1 -o tests/result-5.1-conf.bin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Then read the result back using:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>./wlconf -gcore.hangover.quiet_time -i tests/result-5.1-conf.bin</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Run the following command:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>./wlconf -s core.hangover.quiet_time_1=0x1 -o tests/result-5.2-conf.bin</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Run the following command:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>./wlconf -score.rate.rate_retry_policy=1,2,3,4,5,6,7,8,9,10,11,12 -o tests/result-5.3-conf.bin</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Run the following command:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>./wlconf -score.rate=0x10 -o tests/result-5.4-conf.bin</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Run the following command:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>./wlconf -s core.hangover.quiet_time=aa -o tests/result-5.5-conf.bin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Then read the result back using:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>./wlconf -gcore.hangover.quiet_time -i tests/result-5.5-conf.bin</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Run the following to get configuration from default bin:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>./wlconf -g  &gt; tests/result-4.8-1.conf</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Then write the result back with the following command:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>./wlconf -C tests/result-4.8-1.conf -o tests/result-4.8-conf.bin</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+And read it again:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>./wlconf --get -i tests/result-4.8-conf.bin &gt; tests/result-4.8-2.conf</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Compare the output text configuration files:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">diff -u tests/result-4.8-1.conf tests/result-4.8-2.conf
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Compare the deault and output configuration bin file:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>diff -ua wl18xx-conf-default.bin tests/result-4.8-conf.bin</t>
+    </r>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>6.7</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Remove bin configuration:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rm /system/etc/firmware/ti-connectivity/wl18xx-conf.bin</t>
     </r>
     <r>
       <rPr>
@@ -3610,19 +3712,71 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Run the following command:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>./wlconf -s core.hangover.quiet_time=0x1 -o tests/result-5.1-conf.bin</t>
+      <t xml:space="preserve">Check the influence of changing </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">TX power </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parameter on running system</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Check the influence of changing </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">RTS Threshold </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parameter on running system</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">First run a TX TCP test using Blaze as STA with SISO40 RDL2_RDL4
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Use wireshark to monitor TX power</t>
     </r>
     <r>
       <rPr>
@@ -3633,87 +3787,87 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Then read the result back using:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>./wlconf -gcore.hangover.quiet_time -i tests/result-5.1-conf.bin</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Run the following command:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>./wlconf -s core.hangover.quiet_time_1=0x1 -o tests/result-5.2-conf.bin</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Run the following command:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>./wlconf -score.rate.rate_retry_policy=1,2,3,4,5,6,7,8,9,10,11,12 -o tests/result-5.3-conf.bin</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Run the following command:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>./wlconf -score.rate=0x10 -o tests/result-5.4-conf.bin</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Run the following command:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>./wlconf -s core.hangover.quiet_time=aa -o tests/result-5.5-conf.bin</t>
+Then modify TX power parameter using:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">wlconf -i /system/etc/firmware/ti-connectivity/wl18xx-conf.bin -o /system/etc/firmware/ti-connectivity/wl18xx-conf.bin -s wl18xx.phy.high_power_val=0x0a
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Restart the Driver as STA
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Use wireshark again to monitor TX power</t>
+    </r>
+  </si>
+  <si>
+    <t>There should be a decrease in monitored maximum TX power</t>
+  </si>
+  <si>
+    <t>6.8</t>
+  </si>
+  <si>
+    <t>After changing RTS threshold we should monitor RTS and CTS messages with our TX (1500 bytes) operations</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">wlconf should run the same in multi systems - including with different word sizes, alignment, char signed/unsigned, etc…
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Currently the only limitation is that it should be used only on Little Endian machines (such as ARM and X86)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">First run TX TCP test with frames size 1500 using Blaze as STA with SISO40 RDL2_RDL4
+Use a channel that is currently free of RTS/CTS frames (i.e try using channel 44)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Use wireshark to monitor RTS/CTS</t>
     </r>
     <r>
       <rPr>
@@ -3724,19 +3878,42 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Then read the result back using:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>./wlconf -gcore.hangover.quiet_time -i tests/result-5.5-conf.bin</t>
+Then modify RTS Threshold parameter using:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">wlconf -i /system/etc/firmware/ti-connectivity/wl18xx-conf.bin -o /system/etc/firmware/ti-connectivity/wl18xx-conf.bin -s core.rx.rts_threshold=1000
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Restart the Driver as STA and run the test again
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Use wireshark again to monitor RTS/CTS</t>
     </r>
   </si>
 </sst>
@@ -3744,7 +3921,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3797,6 +3974,23 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -4001,7 +4195,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4052,6 +4246,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4414,10 +4611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:G61"/>
+  <dimension ref="B2:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4453,144 +4650,144 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="47.25" customHeight="1">
-      <c r="B3" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="34"/>
+      <c r="B3" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="35"/>
     </row>
     <row r="4" spans="2:7" ht="60">
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="11">
         <v>1.1000000000000001</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="G4" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="60">
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="12">
         <v>1.2</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="60">
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="12">
         <v>1.3</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="45">
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="12">
         <v>1.4</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="8" spans="2:7" ht="90">
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="12">
         <v>1.5</v>
       </c>
       <c r="E8" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="9" spans="2:7" ht="45">
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="12">
         <v>1.6</v>
       </c>
       <c r="E9" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="10" spans="2:7" ht="90">
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="13">
         <v>1.7</v>
       </c>
       <c r="E10" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>96</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="121.5" customHeight="1">
       <c r="B11" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="31"/>
+        <v>97</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="32"/>
     </row>
     <row r="12" spans="2:7" ht="90">
       <c r="B12" s="3"/>
@@ -4599,13 +4796,13 @@
         <v>1.8</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="90">
@@ -4615,140 +4812,140 @@
         <v>1.9</v>
       </c>
       <c r="E13" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="90">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E14" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>124</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="75">
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
       <c r="D15" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E15" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>165</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="120">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="90">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="G17" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="90">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E18" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G18" s="7" t="s">
         <v>116</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="90">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="13" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E19" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G19" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="F19" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>114</v>
-      </c>
     </row>
     <row r="20" spans="2:7" ht="42" customHeight="1">
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="D20" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="30"/>
+    </row>
+    <row r="21" spans="2:7" ht="18" customHeight="1">
+      <c r="B21" s="24"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="29"/>
-    </row>
-    <row r="21" spans="2:7" ht="18" customHeight="1">
-      <c r="B21" s="23"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="35" t="s">
-        <v>149</v>
-      </c>
-      <c r="E21" s="35"/>
-      <c r="F21" s="36" t="s">
-        <v>148</v>
-      </c>
-      <c r="G21" s="37"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="G21" s="38"/>
     </row>
     <row r="22" spans="2:7" ht="105">
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
       <c r="D22" s="11">
         <v>2.1</v>
       </c>
@@ -4763,8 +4960,8 @@
       </c>
     </row>
     <row r="23" spans="2:7" ht="75">
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
       <c r="D23" s="12">
         <v>2.2000000000000002</v>
       </c>
@@ -4779,8 +4976,8 @@
       </c>
     </row>
     <row r="24" spans="2:7" ht="75">
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="12">
         <v>2.2999999999999998</v>
       </c>
@@ -4795,8 +4992,8 @@
       </c>
     </row>
     <row r="25" spans="2:7" ht="75">
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
       <c r="D25" s="13">
         <v>2.4</v>
       </c>
@@ -4811,34 +5008,34 @@
       </c>
     </row>
     <row r="26" spans="2:7" ht="29.25" customHeight="1">
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="27" t="s">
-        <v>146</v>
-      </c>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="32"/>
+      <c r="D26" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="33"/>
     </row>
     <row r="27" spans="2:7" ht="18" customHeight="1">
-      <c r="B27" s="23"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="35" t="s">
-        <v>149</v>
-      </c>
-      <c r="E27" s="35"/>
-      <c r="F27" s="36" t="s">
-        <v>150</v>
-      </c>
-      <c r="G27" s="37"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="E27" s="36"/>
+      <c r="F27" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="G27" s="38"/>
     </row>
     <row r="28" spans="2:7" ht="135">
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
       <c r="D28" s="11">
         <v>3.1</v>
       </c>
@@ -4853,8 +5050,8 @@
       </c>
     </row>
     <row r="29" spans="2:7" ht="45">
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
       <c r="D29" s="12">
         <v>3.2</v>
       </c>
@@ -4869,8 +5066,8 @@
       </c>
     </row>
     <row r="30" spans="2:7" ht="105">
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
       <c r="D30" s="12">
         <v>3.3</v>
       </c>
@@ -4885,8 +5082,8 @@
       </c>
     </row>
     <row r="31" spans="2:7" ht="60">
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
       <c r="D31" s="12">
         <v>3.4</v>
       </c>
@@ -4901,8 +5098,8 @@
       </c>
     </row>
     <row r="32" spans="2:7" ht="60">
-      <c r="B32" s="23"/>
-      <c r="C32" s="23"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
       <c r="D32" s="12">
         <v>3.5</v>
       </c>
@@ -4913,12 +5110,12 @@
         <v>34</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="45">
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
       <c r="D33" s="13">
         <v>3.6</v>
       </c>
@@ -4933,22 +5130,22 @@
       </c>
     </row>
     <row r="34" spans="2:7" ht="22.5" customHeight="1">
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="21"/>
+      <c r="D34" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="22"/>
     </row>
     <row r="35" spans="2:7" ht="79.5" customHeight="1">
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
       <c r="D35" s="11">
         <v>4.0999999999999996</v>
       </c>
@@ -4963,8 +5160,8 @@
       </c>
     </row>
     <row r="36" spans="2:7" ht="120">
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
       <c r="D36" s="12">
         <v>4.2</v>
       </c>
@@ -4979,8 +5176,8 @@
       </c>
     </row>
     <row r="37" spans="2:7" ht="30">
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="24"/>
       <c r="D37" s="12">
         <v>4.3</v>
       </c>
@@ -4995,8 +5192,8 @@
       </c>
     </row>
     <row r="38" spans="2:7" ht="240">
-      <c r="B38" s="23"/>
-      <c r="C38" s="23"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
       <c r="D38" s="12">
         <v>4.4000000000000004</v>
       </c>
@@ -5011,8 +5208,8 @@
       </c>
     </row>
     <row r="39" spans="2:7" ht="120">
-      <c r="B39" s="23"/>
-      <c r="C39" s="23"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="24"/>
       <c r="D39" s="12">
         <v>4.5</v>
       </c>
@@ -5027,8 +5224,8 @@
       </c>
     </row>
     <row r="40" spans="2:7" ht="120">
-      <c r="B40" s="23"/>
-      <c r="C40" s="23"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24"/>
       <c r="D40" s="12">
         <v>4.5999999999999996</v>
       </c>
@@ -5043,8 +5240,8 @@
       </c>
     </row>
     <row r="41" spans="2:7" ht="60">
-      <c r="B41" s="23"/>
-      <c r="C41" s="23"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
       <c r="D41" s="12">
         <v>4.7</v>
       </c>
@@ -5052,269 +5249,293 @@
         <v>58</v>
       </c>
       <c r="F41" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="G41" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G41" s="7" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="42" spans="2:7" ht="150">
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
       <c r="D42" s="13">
         <v>4.8</v>
       </c>
       <c r="E42" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="G42" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="F42" s="8" t="s">
+    </row>
+    <row r="43" spans="2:7" ht="30.75" customHeight="1">
+      <c r="B43" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="G42" s="14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" ht="30.75" customHeight="1">
-      <c r="B43" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C43" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="21"/>
+      <c r="D43" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="22"/>
     </row>
     <row r="44" spans="2:7" ht="60">
-      <c r="B44" s="23"/>
-      <c r="C44" s="23"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="24"/>
       <c r="D44" s="11">
         <v>5.0999999999999996</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="2:7" ht="45">
-      <c r="B45" s="23"/>
-      <c r="C45" s="23"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="24"/>
       <c r="D45" s="12">
         <v>5.2</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="2:7" ht="45">
-      <c r="B46" s="23"/>
-      <c r="C46" s="23"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
       <c r="D46" s="12">
         <v>5.3</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="2:7" ht="45">
-      <c r="B47" s="23"/>
-      <c r="C47" s="23"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="24"/>
       <c r="D47" s="12">
         <v>5.4</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="2:7" ht="60">
-      <c r="B48" s="23"/>
-      <c r="C48" s="23"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="24"/>
       <c r="D48" s="12">
         <v>5.5</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="2:7" ht="75">
-      <c r="B49" s="24"/>
-      <c r="C49" s="24"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
       <c r="D49" s="12">
         <v>5.6</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="15" customHeight="1">
-      <c r="B50" s="22" t="s">
+      <c r="B50" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="C50" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="22"/>
+    </row>
+    <row r="51" spans="2:7" ht="90">
+      <c r="B51" s="24"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="165">
+      <c r="B52" s="24"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="G52" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C50" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="D50" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="21"/>
-    </row>
-    <row r="51" spans="2:7" ht="90">
-      <c r="B51" s="23"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="12" t="s">
+    </row>
+    <row r="53" spans="2:7" ht="165">
+      <c r="B53" s="24"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="E51" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="F51" s="6" t="s">
+      <c r="E53" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" ht="180">
+      <c r="B54" s="24"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="G51" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7" ht="165">
-      <c r="B52" s="23"/>
-      <c r="C52" s="26"/>
-      <c r="D52" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="G52" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7" ht="165">
-      <c r="B53" s="23"/>
-      <c r="C53" s="26"/>
-      <c r="D53" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="E53" s="6" t="s">
+      <c r="E54" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F54" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="F53" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="G53" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7" ht="180">
-      <c r="B54" s="23"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="12" t="s">
+      <c r="G54" s="7" t="s">
         <v>139</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="G54" s="7" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="55" spans="2:7" ht="165">
       <c r="B55" s="24"/>
-      <c r="C55" s="38"/>
+      <c r="C55" s="27"/>
       <c r="D55" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="G55" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="E55" s="8" t="s">
+    </row>
+    <row r="56" spans="2:7" ht="120">
+      <c r="B56" s="24"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="G56" s="14" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" ht="117.75" customHeight="1">
+      <c r="B57" s="25"/>
+      <c r="C57" s="39"/>
+      <c r="D57" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="G57" s="14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" ht="30.75" customHeight="1">
+      <c r="B58" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="C58" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="F55" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="G55" s="14" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" ht="30.75" customHeight="1">
-      <c r="B56" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="C56" s="18" t="s">
+      <c r="D58" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="22"/>
+    </row>
+    <row r="59" spans="2:7" ht="75">
+      <c r="B59" s="20"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F59" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="D56" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="E56" s="20"/>
-      <c r="F56" s="20"/>
-      <c r="G56" s="21"/>
-    </row>
-    <row r="57" spans="2:7" ht="75">
-      <c r="B57" s="19"/>
-      <c r="C57" s="19"/>
-      <c r="D57" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="E57" s="5" t="s">
+      <c r="G59" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="F57" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="G57" s="17" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7">
-      <c r="B58" s="9"/>
-      <c r="D58" s="1"/>
-    </row>
-    <row r="59" spans="2:7">
-      <c r="B59" s="9"/>
-      <c r="D59" s="1"/>
     </row>
     <row r="60" spans="2:7">
       <c r="B60" s="9"/>
@@ -5324,10 +5545,18 @@
       <c r="B61" s="9"/>
       <c r="D61" s="1"/>
     </row>
+    <row r="62" spans="2:7">
+      <c r="B62" s="9"/>
+      <c r="D62" s="1"/>
+    </row>
+    <row r="63" spans="2:7">
+      <c r="B63" s="9"/>
+      <c r="D63" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="26">
     <mergeCell ref="F27:G27"/>
-    <mergeCell ref="B50:B55"/>
+    <mergeCell ref="B50:B57"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="D34:G34"/>
@@ -5335,10 +5564,10 @@
     <mergeCell ref="B43:B49"/>
     <mergeCell ref="D43:G43"/>
     <mergeCell ref="D50:G50"/>
-    <mergeCell ref="C50:C55"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="C50:C57"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="D58:G58"/>
     <mergeCell ref="B3:B10"/>
     <mergeCell ref="C20:C25"/>
     <mergeCell ref="B20:B25"/>

</xml_diff>

<commit_message>
wlconf: add support for recovery setting conf
add support for recovery settings conf including bug_on_recovery
and no_recovery options. This aligns with latest kernel change.

In addition to updating conf.h, the following files were regenerated:
struct.bin
default.conf
example.conf
wl18xx-cond-default.bin

Also tests were updated in accordance to the change and a small error
in wlconf_unit_test.xlsx was fixed.

Signed-off-by: Yair Shapira <yair.shapira@ti.com>
</commit_message>
<xml_diff>
--- a/wlconf/tests/wlconf_unit_test.xlsx
+++ b/wlconf/tests/wlconf_unit_test.xlsx
@@ -3617,9 +3617,6 @@
     </r>
   </si>
   <si>
-    <t>sdf</t>
-  </si>
-  <si>
     <t>6.7</t>
   </si>
   <si>
@@ -3914,6 +3911,46 @@
         <scheme val="minor"/>
       </rPr>
       <t>Use wireshark again to monitor RTS/CTS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Run the following command:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>./wlconf -p &gt; tests/result-4.7.struct</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Then check that the output matches the pre-defined one:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>diff -u tests/result-4.7.struct tests/test-4.7.struct</t>
     </r>
   </si>
 </sst>
@@ -4251,16 +4288,10 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4272,10 +4303,28 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4297,18 +4346,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4613,8 +4650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4650,22 +4687,22 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="47.25" customHeight="1">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="39"/>
     </row>
     <row r="4" spans="2:7" ht="60">
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="11">
         <v>1.1000000000000001</v>
       </c>
@@ -4680,8 +4717,8 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="60">
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="12">
         <v>1.2</v>
       </c>
@@ -4696,8 +4733,8 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="60">
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
       <c r="D6" s="12">
         <v>1.3</v>
       </c>
@@ -4712,8 +4749,8 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="45">
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="12">
         <v>1.4</v>
       </c>
@@ -4728,8 +4765,8 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="90">
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="12">
         <v>1.5</v>
       </c>
@@ -4744,8 +4781,8 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="45">
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
       <c r="D9" s="12">
         <v>1.6</v>
       </c>
@@ -4760,8 +4797,8 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="90">
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="13">
         <v>1.7</v>
       </c>
@@ -4782,12 +4819,12 @@
       <c r="C11" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="32"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="36"/>
     </row>
     <row r="12" spans="2:7" ht="90">
       <c r="B12" s="3"/>
@@ -4918,34 +4955,34 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="42" customHeight="1">
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="30"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="34"/>
     </row>
     <row r="21" spans="2:7" ht="18" customHeight="1">
-      <c r="B21" s="24"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="36" t="s">
+      <c r="B21" s="22"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="E21" s="36"/>
-      <c r="F21" s="37" t="s">
+      <c r="E21" s="24"/>
+      <c r="F21" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="G21" s="38"/>
+      <c r="G21" s="20"/>
     </row>
     <row r="22" spans="2:7" ht="105">
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
       <c r="D22" s="11">
         <v>2.1</v>
       </c>
@@ -4960,8 +4997,8 @@
       </c>
     </row>
     <row r="23" spans="2:7" ht="75">
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
       <c r="D23" s="12">
         <v>2.2000000000000002</v>
       </c>
@@ -4976,8 +5013,8 @@
       </c>
     </row>
     <row r="24" spans="2:7" ht="75">
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
       <c r="D24" s="12">
         <v>2.2999999999999998</v>
       </c>
@@ -4992,8 +5029,8 @@
       </c>
     </row>
     <row r="25" spans="2:7" ht="75">
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
       <c r="D25" s="13">
         <v>2.4</v>
       </c>
@@ -5008,34 +5045,34 @@
       </c>
     </row>
     <row r="26" spans="2:7" ht="29.25" customHeight="1">
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="33"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="37"/>
     </row>
     <row r="27" spans="2:7" ht="18" customHeight="1">
-      <c r="B27" s="24"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="36" t="s">
+      <c r="B27" s="22"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="E27" s="36"/>
-      <c r="F27" s="37" t="s">
+      <c r="E27" s="24"/>
+      <c r="F27" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="G27" s="38"/>
+      <c r="G27" s="20"/>
     </row>
     <row r="28" spans="2:7" ht="135">
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
       <c r="D28" s="11">
         <v>3.1</v>
       </c>
@@ -5050,8 +5087,8 @@
       </c>
     </row>
     <row r="29" spans="2:7" ht="45">
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
       <c r="D29" s="12">
         <v>3.2</v>
       </c>
@@ -5066,8 +5103,8 @@
       </c>
     </row>
     <row r="30" spans="2:7" ht="105">
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
       <c r="D30" s="12">
         <v>3.3</v>
       </c>
@@ -5082,8 +5119,8 @@
       </c>
     </row>
     <row r="31" spans="2:7" ht="60">
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
       <c r="D31" s="12">
         <v>3.4</v>
       </c>
@@ -5098,8 +5135,8 @@
       </c>
     </row>
     <row r="32" spans="2:7" ht="60">
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
       <c r="D32" s="12">
         <v>3.5</v>
       </c>
@@ -5114,8 +5151,8 @@
       </c>
     </row>
     <row r="33" spans="2:7" ht="45">
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
       <c r="D33" s="13">
         <v>3.6</v>
       </c>
@@ -5130,22 +5167,22 @@
       </c>
     </row>
     <row r="34" spans="2:7" ht="22.5" customHeight="1">
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="26" t="s">
+      <c r="C34" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="21" t="s">
+      <c r="D34" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="22"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="26"/>
     </row>
     <row r="35" spans="2:7" ht="79.5" customHeight="1">
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
       <c r="D35" s="11">
         <v>4.0999999999999996</v>
       </c>
@@ -5160,8 +5197,8 @@
       </c>
     </row>
     <row r="36" spans="2:7" ht="120">
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
       <c r="D36" s="12">
         <v>4.2</v>
       </c>
@@ -5176,8 +5213,8 @@
       </c>
     </row>
     <row r="37" spans="2:7" ht="30">
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
       <c r="D37" s="12">
         <v>4.3</v>
       </c>
@@ -5192,8 +5229,8 @@
       </c>
     </row>
     <row r="38" spans="2:7" ht="240">
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
       <c r="D38" s="12">
         <v>4.4000000000000004</v>
       </c>
@@ -5208,8 +5245,8 @@
       </c>
     </row>
     <row r="39" spans="2:7" ht="120">
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
       <c r="D39" s="12">
         <v>4.5</v>
       </c>
@@ -5224,8 +5261,8 @@
       </c>
     </row>
     <row r="40" spans="2:7" ht="120">
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
       <c r="D40" s="12">
         <v>4.5999999999999996</v>
       </c>
@@ -5240,8 +5277,8 @@
       </c>
     </row>
     <row r="41" spans="2:7" ht="60">
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
       <c r="D41" s="12">
         <v>4.7</v>
       </c>
@@ -5249,15 +5286,15 @@
         <v>58</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="G41" s="7" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="42" spans="2:7" ht="150">
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
       <c r="D42" s="13">
         <v>4.8</v>
       </c>
@@ -5272,22 +5309,22 @@
       </c>
     </row>
     <row r="43" spans="2:7" ht="30.75" customHeight="1">
-      <c r="B43" s="23" t="s">
+      <c r="B43" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C43" s="26" t="s">
+      <c r="C43" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="D43" s="21" t="s">
+      <c r="D43" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="E43" s="21"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="22"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="26"/>
     </row>
     <row r="44" spans="2:7" ht="60">
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
       <c r="D44" s="11">
         <v>5.0999999999999996</v>
       </c>
@@ -5302,8 +5339,8 @@
       </c>
     </row>
     <row r="45" spans="2:7" ht="45">
-      <c r="B45" s="24"/>
-      <c r="C45" s="24"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="22"/>
       <c r="D45" s="12">
         <v>5.2</v>
       </c>
@@ -5318,8 +5355,8 @@
       </c>
     </row>
     <row r="46" spans="2:7" ht="45">
-      <c r="B46" s="24"/>
-      <c r="C46" s="24"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
       <c r="D46" s="12">
         <v>5.3</v>
       </c>
@@ -5334,8 +5371,8 @@
       </c>
     </row>
     <row r="47" spans="2:7" ht="45">
-      <c r="B47" s="24"/>
-      <c r="C47" s="24"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
       <c r="D47" s="12">
         <v>5.4</v>
       </c>
@@ -5350,8 +5387,8 @@
       </c>
     </row>
     <row r="48" spans="2:7" ht="60">
-      <c r="B48" s="24"/>
-      <c r="C48" s="24"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="22"/>
       <c r="D48" s="12">
         <v>5.5</v>
       </c>
@@ -5366,8 +5403,8 @@
       </c>
     </row>
     <row r="49" spans="2:7" ht="75">
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
       <c r="D49" s="12">
         <v>5.6</v>
       </c>
@@ -5382,22 +5419,22 @@
       </c>
     </row>
     <row r="50" spans="2:7" ht="15" customHeight="1">
-      <c r="B50" s="23" t="s">
+      <c r="B50" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="C50" s="26" t="s">
+      <c r="C50" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="D50" s="21" t="s">
+      <c r="D50" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="22"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="25"/>
+      <c r="G50" s="26"/>
     </row>
     <row r="51" spans="2:7" ht="90">
-      <c r="B51" s="24"/>
-      <c r="C51" s="27"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="28"/>
       <c r="D51" s="12" t="s">
         <v>126</v>
       </c>
@@ -5412,8 +5449,8 @@
       </c>
     </row>
     <row r="52" spans="2:7" ht="165">
-      <c r="B52" s="24"/>
-      <c r="C52" s="27"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="28"/>
       <c r="D52" s="12" t="s">
         <v>127</v>
       </c>
@@ -5428,8 +5465,8 @@
       </c>
     </row>
     <row r="53" spans="2:7" ht="165">
-      <c r="B53" s="24"/>
-      <c r="C53" s="27"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="28"/>
       <c r="D53" s="12" t="s">
         <v>128</v>
       </c>
@@ -5444,8 +5481,8 @@
       </c>
     </row>
     <row r="54" spans="2:7" ht="180">
-      <c r="B54" s="24"/>
-      <c r="C54" s="27"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="28"/>
       <c r="D54" s="12" t="s">
         <v>137</v>
       </c>
@@ -5460,8 +5497,8 @@
       </c>
     </row>
     <row r="55" spans="2:7" ht="165">
-      <c r="B55" s="24"/>
-      <c r="C55" s="27"/>
+      <c r="B55" s="22"/>
+      <c r="C55" s="28"/>
       <c r="D55" s="13" t="s">
         <v>141</v>
       </c>
@@ -5469,63 +5506,63 @@
         <v>154</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G55" s="14" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="56" spans="2:7" ht="120">
-      <c r="B56" s="24"/>
-      <c r="C56" s="27"/>
+      <c r="B56" s="22"/>
+      <c r="C56" s="28"/>
       <c r="D56" s="13" t="s">
         <v>155</v>
       </c>
       <c r="E56" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="G56" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" ht="117.75" customHeight="1">
+      <c r="B57" s="23"/>
+      <c r="C57" s="29"/>
+      <c r="D57" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="E57" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="F56" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="G56" s="14" t="s">
+      <c r="F57" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="G57" s="14" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" ht="30.75" customHeight="1">
+      <c r="B58" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="C58" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="D58" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="E58" s="25"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="26"/>
+    </row>
+    <row r="59" spans="2:7" ht="75">
+      <c r="B59" s="31"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="11" t="s">
         <v>178</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7" ht="117.75" customHeight="1">
-      <c r="B57" s="25"/>
-      <c r="C57" s="39"/>
-      <c r="D57" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="E57" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="F57" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="G57" s="14" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" ht="30.75" customHeight="1">
-      <c r="B58" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="C58" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="D58" s="21" t="s">
-        <v>181</v>
-      </c>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
-      <c r="G58" s="22"/>
-    </row>
-    <row r="59" spans="2:7" ht="75">
-      <c r="B59" s="20"/>
-      <c r="C59" s="20"/>
-      <c r="D59" s="11" t="s">
-        <v>179</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>157</v>
@@ -5555,16 +5592,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="B50:B57"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="B43:B49"/>
-    <mergeCell ref="D43:G43"/>
-    <mergeCell ref="D50:G50"/>
-    <mergeCell ref="C50:C57"/>
     <mergeCell ref="C58:C59"/>
     <mergeCell ref="B58:B59"/>
     <mergeCell ref="D58:G58"/>
@@ -5581,6 +5608,16 @@
     <mergeCell ref="D3:G3"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="B50:B57"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="B43:B49"/>
+    <mergeCell ref="D43:G43"/>
+    <mergeCell ref="D50:G50"/>
+    <mergeCell ref="C50:C57"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F27:G27" r:id="rId1" display="example.ini"/>

</xml_diff>